<commit_message>
set constraint on GLD in basic_asset_classes_unconstrained to 100%
</commit_message>
<xml_diff>
--- a/data/1_basic_asset_classes_unconstrained.xlsx
+++ b/data/1_basic_asset_classes_unconstrained.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6113f60f932799a7/1Evan/.efficient_frontier/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{89F79A55-B33C-47ED-B201-06C3BCCC6DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E54AF128-6B3F-404B-A139-38DD82592D95}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{89F79A55-B33C-47ED-B201-06C3BCCC6DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2191C200-786F-41A1-B8F4-8095EDF8C3E9}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00%"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -135,7 +135,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -153,6 +153,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -446,7 +450,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -545,7 +549,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="6">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>